<commit_message>
A couple various tweaks to simplify the UI
</commit_message>
<xml_diff>
--- a/Parameter Explanations Old.xlsx
+++ b/Parameter Explanations Old.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Personal Study\Programming\disco-diffusion-dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28666A3A-4406-4D19-BE94-ED864DD00808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBACA466-A601-4C70-93D0-8486BFAC73E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24375" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -967,14 +967,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C74" sqref="C74"/>
+      <selection pane="bottomRight" activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,7 +1011,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1026,7 +1025,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1036,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1065,7 +1064,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1079,7 +1078,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1093,7 +1092,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1107,7 +1106,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1124,7 +1123,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1141,7 +1140,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1152,7 +1151,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -1175,7 +1174,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -1189,7 +1188,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1206,7 +1205,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -1220,7 +1219,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -1234,7 +1233,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -1248,7 +1247,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1265,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1282,7 +1281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1299,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1319,7 +1318,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1339,7 +1338,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1359,7 +1358,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1376,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1396,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1416,7 +1415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1610,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -1633,7 +1632,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -1653,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1673,7 +1672,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -1690,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -1707,7 +1706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -1724,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -1741,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1758,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1775,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -1792,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1809,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1826,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -1860,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -1883,7 +1882,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -1903,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -1923,7 +1922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -1940,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -1957,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>33</v>
       </c>
@@ -1980,7 +1979,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>27</v>
       </c>
@@ -1997,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>50</v>
       </c>
@@ -2017,7 +2016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>28</v>
       </c>
@@ -2037,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -2091,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -2111,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -2128,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -2148,7 +2147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -2165,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -2182,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -2199,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -2216,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -2233,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>34</v>
       </c>
@@ -2253,7 +2252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>52</v>
       </c>
@@ -2273,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>54</v>
       </c>
@@ -2313,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -2332,11 +2331,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H75" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="model"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H17">
       <sortCondition ref="A1:A75"/>
     </sortState>

</xml_diff>